<commit_message>
Paciente no valido eliminado de the only excel
</commit_message>
<xml_diff>
--- a/resources/the_only_excel.xlsx
+++ b/resources/the_only_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Universidad\Workspace\TFG-UroAnalytics\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692F5C9A-4501-4685-8B69-E5B0ABC2CBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA7746E-1E9B-4028-BDAC-EFE3F2CE59C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,9 +742,16 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1075,170 +1082,171 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1520,7 +1528,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:BP270"/>
+  <dimension ref="A1:BP271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B256" activePane="bottomRight" state="frozen"/>
@@ -52649,6 +52657,70 @@
         <v>0.00</v>
       </c>
     </row>
+    <row r="271" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A271" s="57"/>
+      <c r="B271" s="58"/>
+      <c r="C271" s="97"/>
+      <c r="D271" s="57"/>
+      <c r="E271" s="97"/>
+      <c r="F271" s="57"/>
+      <c r="G271" s="57"/>
+      <c r="H271" s="57"/>
+      <c r="I271" s="57"/>
+      <c r="J271" s="57"/>
+      <c r="K271" s="57"/>
+      <c r="L271" s="57"/>
+      <c r="M271" s="57"/>
+      <c r="N271" s="57"/>
+      <c r="O271" s="57"/>
+      <c r="P271" s="57"/>
+      <c r="Q271" s="57"/>
+      <c r="R271" s="57"/>
+      <c r="S271" s="57"/>
+      <c r="T271" s="57"/>
+      <c r="U271" s="57"/>
+      <c r="V271" s="57"/>
+      <c r="W271" s="57"/>
+      <c r="X271" s="57"/>
+      <c r="Y271" s="57"/>
+      <c r="Z271" s="57"/>
+      <c r="AA271" s="57"/>
+      <c r="AB271" s="57"/>
+      <c r="AC271" s="57"/>
+      <c r="AD271" s="57"/>
+      <c r="AE271" s="57"/>
+      <c r="AF271" s="57"/>
+      <c r="AG271" s="57"/>
+      <c r="AH271" s="57"/>
+      <c r="AI271" s="57"/>
+      <c r="AJ271" s="57"/>
+      <c r="AK271" s="57"/>
+      <c r="AL271" s="57"/>
+      <c r="AM271" s="57"/>
+      <c r="AN271" s="57"/>
+      <c r="AO271" s="57"/>
+      <c r="AP271" s="76"/>
+      <c r="AQ271" s="57"/>
+      <c r="AR271" s="57"/>
+      <c r="AS271" s="79"/>
+      <c r="AT271" s="57"/>
+      <c r="AU271" s="58"/>
+      <c r="AV271" s="67"/>
+      <c r="AW271" s="57"/>
+      <c r="AX271" s="57"/>
+      <c r="AY271" s="57"/>
+      <c r="AZ271" s="57"/>
+      <c r="BA271" s="57"/>
+      <c r="BB271" s="57"/>
+      <c r="BC271" s="57"/>
+      <c r="BD271" s="57"/>
+      <c r="BE271" s="57"/>
+      <c r="BF271" s="57"/>
+      <c r="BG271" s="57"/>
+      <c r="BH271" s="57"/>
+      <c r="BI271" s="57"/>
+      <c r="BJ271" s="57"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>